<commit_message>
Add Create Patient and Doctor endpoints
Adding the endpoints to create a new doctor and a new patient
</commit_message>
<xml_diff>
--- a/TestAccountPasswords.xlsx
+++ b/TestAccountPasswords.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matt W\source\repos\ABC_Hospital_Web_Service\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Matt W\Documents\GitHub\hospitalmanagement\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A7F83ED2-0F85-408C-B8B2-F8BC9CC7A305}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28CB86A1-EB25-4750-8F14-D59F8CD08E8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{83371B51-3C5D-4CB4-939A-CA7136549D19}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{83371B51-3C5D-4CB4-939A-CA7136549D19}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
   <si>
     <t>Username</t>
   </si>
@@ -129,6 +129,18 @@
   </si>
   <si>
     <t>testersGottaTest</t>
+  </si>
+  <si>
+    <t>qcee1</t>
+  </si>
+  <si>
+    <t>RustyIsMyDog</t>
+  </si>
+  <si>
+    <t>ecee1</t>
+  </si>
+  <si>
+    <t>RustyIsActuallyMyDog</t>
   </si>
 </sst>
 </file>
@@ -162,7 +174,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -194,14 +206,25 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -209,6 +232,13 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -524,10 +554,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB13014B-428E-4D86-B3DF-90B17171FE09}">
-  <dimension ref="A1:C16"/>
+  <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -556,7 +586,7 @@
         <v>18</v>
       </c>
       <c r="C2" s="2" t="str">
-        <f t="shared" ref="C2:C16" si="0">"{" &amp; CHAR(34) &amp; "username" &amp; CHAR(34) &amp; ":" &amp; CHAR(34) &amp; A2 &amp; CHAR(34) &amp; "," &amp; CHAR(34) &amp; "password" &amp; CHAR(34) &amp; ":" &amp; CHAR(34) &amp; B2 &amp; CHAR(34) &amp; "}"</f>
+        <f t="shared" ref="C2:C18" si="0">"{" &amp; CHAR(34) &amp; "username" &amp; CHAR(34) &amp; ":" &amp; CHAR(34) &amp; A2 &amp; CHAR(34) &amp; "," &amp; CHAR(34) &amp; "password" &amp; CHAR(34) &amp; ":" &amp; CHAR(34) &amp; B2 &amp; CHAR(34) &amp; "}"</f>
         <v>{"username":"aadmin1","password":"ABCDmin2023"}</v>
       </c>
     </row>
@@ -726,6 +756,30 @@
       <c r="C16" s="2" t="str">
         <f t="shared" si="0"/>
         <v>{"username":"smurray2","password":"aquamarine2023"}</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C17" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>{"username":"qcee1","password":"RustyIsMyDog"}</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C18" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>{"username":"ecee1","password":"RustyIsActuallyMyDog"}</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Performing some final cleanup
Removing some debugging lines of code and uploading the most recent version of the database to prepare for submission
</commit_message>
<xml_diff>
--- a/TestAccountPasswords.xlsx
+++ b/TestAccountPasswords.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Matt W\Documents\GitHub\hospitalmanagement\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Matt W\Documents\GitHub\hospitalmanagement2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28CB86A1-EB25-4750-8F14-D59F8CD08E8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB4F3BD1-FBE9-4FBB-BB2B-EBBEB364A78E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{83371B51-3C5D-4CB4-939A-CA7136549D19}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
   <si>
     <t>Username</t>
   </si>
@@ -113,9 +113,6 @@
     <t>BreathOfTheWild:)</t>
   </si>
   <si>
-    <t>Json</t>
-  </si>
-  <si>
     <t>pa55w0rd</t>
   </si>
   <si>
@@ -141,6 +138,24 @@
   </si>
   <si>
     <t>RustyIsActuallyMyDog</t>
+  </si>
+  <si>
+    <t>jhess1</t>
+  </si>
+  <si>
+    <t>examplePatient</t>
+  </si>
+  <si>
+    <t>hphilips1</t>
+  </si>
+  <si>
+    <t>exampleDoctor</t>
+  </si>
+  <si>
+    <t>ahill1</t>
+  </si>
+  <si>
+    <t>exampleAdmin</t>
   </si>
 </sst>
 </file>
@@ -174,7 +189,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -206,39 +221,20 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -554,10 +550,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB13014B-428E-4D86-B3DF-90B17171FE09}">
-  <dimension ref="A1:C18"/>
+  <dimension ref="A1:B27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -567,220 +563,197 @@
     <col min="3" max="3" width="52.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="2" t="str">
-        <f t="shared" ref="C2:C18" si="0">"{" &amp; CHAR(34) &amp; "username" &amp; CHAR(34) &amp; ":" &amp; CHAR(34) &amp; A2 &amp; CHAR(34) &amp; "," &amp; CHAR(34) &amp; "password" &amp; CHAR(34) &amp; ":" &amp; CHAR(34) &amp; B2 &amp; CHAR(34) &amp; "}"</f>
-        <v>{"username":"aadmin1","password":"ABCDmin2023"}</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C3" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>{"username":"bjohnson1","password":"password"}</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C4" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>{"username":"dlink1","password":"Will Arnet"}</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C5" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>{"username":"emurray1","password":"#AmAMom"}</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="3">
+      <c r="B6" s="2">
         <v>123456789</v>
       </c>
-      <c r="C6" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>{"username":"jdoe1","password":"123456789"}</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="3">
+      <c r="B7" s="2">
         <v>234567890</v>
       </c>
-      <c r="C7" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>{"username":"jdoe2","password":"234567890"}</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="C8" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>{"username":"jtesting1","password":"testersGottaTest"}</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B8" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="C9" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>{"username":"jupdegra1","password":"TigersGonnaWin"}</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B9" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="C10" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>{"username":"jupdegra2","password":"IAmGroot!"}</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B10" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B11" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C11" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>{"username":"mclement","password":"C#BestLang.py"}</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B11" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B12" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="C12" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>{"username":"mfernand1","password":"pa55w0rd"}</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B12" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="B13" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C13" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>{"username":"slink1","password":"BreathOfTheWild:)"}</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B14" s="3" t="s">
+      <c r="B14" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C14" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>{"username":"slopes1","password":"4theKids"}</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B15" s="3" t="s">
+      <c r="B15" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C15" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>{"username":"smurray1","password":"BatmanIsTheBest"}</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B16" s="3" t="s">
+      <c r="B16" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C16" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>{"username":"smurray2","password":"aquamarine2023"}</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="5" t="s">
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B17" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B17" s="6" t="s">
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C17" s="7" t="str">
-        <f t="shared" si="0"/>
-        <v>{"username":"qcee1","password":"RustyIsMyDog"}</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="5" t="s">
+      <c r="B18" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B18" s="6" t="s">
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C18" s="7" t="str">
-        <f t="shared" si="0"/>
-        <v>{"username":"ecee1","password":"RustyIsActuallyMyDog"}</v>
-      </c>
+      <c r="B19" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="1"/>
+      <c r="B22" s="2"/>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="1"/>
+      <c r="B23" s="2"/>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="1"/>
+      <c r="B24" s="2"/>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="1"/>
+      <c r="B25" s="2"/>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="1"/>
+      <c r="B26" s="2"/>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="1"/>
+      <c r="B27" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>